<commit_message>
bab 2 done, bab 3 design sistem blm, bab 4 - bab 5 done, listing code done, daftar pustaka blm
</commit_message>
<xml_diff>
--- a/tabel implementasi.xlsx
+++ b/tabel implementasi.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tata\JOKI\Joki Feri UPB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80661856-71D2-4B2D-BA1F-F6D38F194300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12923013-7879-44EE-B85C-7628AEBC87F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" xr2:uid="{ED87AB0D-2DF3-4699-9BFA-4F9F6E9FEBF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{ED87AB0D-2DF3-4699-9BFA-4F9F6E9FEBF7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Implementasi" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="81">
   <si>
     <t>Login</t>
   </si>
@@ -239,13 +240,52 @@
   </si>
   <si>
     <t>Data tampil dihalaman Data Report PO</t>
+  </si>
+  <si>
+    <t>No Literatur</t>
+  </si>
+  <si>
+    <t>Penulis</t>
+  </si>
+  <si>
+    <t>Tahun</t>
+  </si>
+  <si>
+    <t>Judul</t>
+  </si>
+  <si>
+    <t>Literatur 1</t>
+  </si>
+  <si>
+    <t>Nur, Hidayat Muhammad</t>
+  </si>
+  <si>
+    <t>Sistem Informasi Service dan Penjualan Sparepart Motor Yamaha Pada PD Enggal Jaya Motor Cikarang Barat</t>
+  </si>
+  <si>
+    <t>Literatur 2</t>
+  </si>
+  <si>
+    <t>Setiadi, Nugraha dan Setiawan, Ridwan</t>
+  </si>
+  <si>
+    <t>Pengembangan Aplikasi Penjualan Sparepart Di Bengkel Anugrah Jaya Motor Berbasis Desktop</t>
+  </si>
+  <si>
+    <t>Literatur 3</t>
+  </si>
+  <si>
+    <t>Welim, Yohannes Yahya</t>
+  </si>
+  <si>
+    <t>Pengembangan Sistem Informasi Service Kendaraan Pada Bengkel KFMP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +301,13 @@
       <family val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -308,18 +355,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -638,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFD4FAA-0F2F-4638-9C66-C2D14B4B6372}">
   <dimension ref="C3:H128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E124" sqref="E124"/>
+    <sheetView topLeftCell="A115" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -658,53 +708,53 @@
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="4" t="s">
+      <c r="G7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D8" s="4">
-        <v>2</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="G8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -714,36 +764,36 @@
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="D15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="4">
-        <v>1</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="4" t="s">
+      <c r="G16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -753,138 +803,138 @@
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23" s="3" t="s">
+      <c r="D23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D24" s="4">
-        <v>1</v>
-      </c>
-      <c r="E24" s="4" t="s">
+      <c r="D24" s="3">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" s="4" t="s">
+      <c r="G24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D25" s="4">
-        <v>2</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="D25" s="3">
+        <v>2</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="4" t="s">
+      <c r="G25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="4">
-        <v>3</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="D26" s="3">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="4" t="s">
+      <c r="G26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <v>4</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="4" t="s">
+      <c r="G27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D28" s="4">
+      <c r="D28" s="3">
         <v>5</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="4" t="s">
+      <c r="G28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D29" s="4">
+      <c r="D29" s="3">
         <v>6</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="4" t="s">
+      <c r="G29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>7</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" s="4" t="s">
+      <c r="G30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -894,121 +944,121 @@
       </c>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D36" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G36" s="3" t="s">
+      <c r="D36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D37" s="4">
-        <v>1</v>
-      </c>
-      <c r="E37" s="4" t="s">
+      <c r="D37" s="3">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H37" s="4" t="s">
+      <c r="G37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D38" s="4">
-        <v>2</v>
-      </c>
-      <c r="E38" s="4" t="s">
+      <c r="D38" s="3">
+        <v>2</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G38" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38" s="4" t="s">
+      <c r="G38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D39" s="4">
-        <v>3</v>
-      </c>
-      <c r="E39" s="4" t="s">
+      <c r="D39" s="3">
+        <v>3</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H39" s="4" t="s">
+      <c r="G39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D40" s="4">
+      <c r="D40" s="3">
         <v>4</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G40" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H40" s="4" t="s">
+      <c r="G40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D41" s="4">
+      <c r="D41" s="3">
         <v>5</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G41" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H41" s="4" t="s">
+      <c r="G41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D42" s="4">
+      <c r="D42" s="3">
         <v>6</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H42" s="4" t="s">
+      <c r="G42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1018,121 +1068,121 @@
       </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D46" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G46" s="3" t="s">
+      <c r="D46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H46" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D47" s="4">
-        <v>1</v>
-      </c>
-      <c r="E47" s="4" t="s">
+      <c r="D47" s="3">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="F47" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G47" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H47" s="4" t="s">
+      <c r="G47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D48" s="4">
-        <v>2</v>
-      </c>
-      <c r="E48" s="4" t="s">
+      <c r="D48" s="3">
+        <v>2</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F48" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G48" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H48" s="4" t="s">
+      <c r="G48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D49" s="4">
-        <v>3</v>
-      </c>
-      <c r="E49" s="4" t="s">
+      <c r="D49" s="3">
+        <v>3</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="F49" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G49" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H49" s="4" t="s">
+      <c r="G49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D50" s="4">
+      <c r="D50" s="3">
         <v>4</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F50" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G50" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H50" s="4" t="s">
+      <c r="G50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H50" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D51" s="4">
+      <c r="D51" s="3">
         <v>5</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F51" s="4" t="s">
+      <c r="F51" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G51" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H51" s="4" t="s">
+      <c r="G51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H51" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D52" s="4">
+      <c r="D52" s="3">
         <v>6</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="F52" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G52" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H52" s="4" t="s">
+      <c r="G52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H52" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1142,121 +1192,121 @@
       </c>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D59" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G59" s="3" t="s">
+      <c r="D59" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G59" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H59" s="3" t="s">
+      <c r="H59" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D60" s="4">
-        <v>1</v>
-      </c>
-      <c r="E60" s="4" t="s">
+      <c r="D60" s="3">
+        <v>1</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F60" s="4" t="s">
+      <c r="F60" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G60" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H60" s="4" t="s">
+      <c r="G60" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H60" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="61" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D61" s="4">
-        <v>2</v>
-      </c>
-      <c r="E61" s="4" t="s">
+      <c r="D61" s="3">
+        <v>2</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F61" s="4" t="s">
+      <c r="F61" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G61" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H61" s="4" t="s">
+      <c r="G61" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H61" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D62" s="4">
-        <v>3</v>
-      </c>
-      <c r="E62" s="4" t="s">
+      <c r="D62" s="3">
+        <v>3</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="F62" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G62" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H62" s="4" t="s">
+      <c r="G62" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H62" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D63" s="4">
+      <c r="D63" s="3">
         <v>4</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="F63" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G63" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H63" s="4" t="s">
+      <c r="G63" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H63" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="64" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D64" s="4">
+      <c r="D64" s="3">
         <v>5</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E64" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F64" s="4" t="s">
+      <c r="F64" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G64" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H64" s="4" t="s">
+      <c r="G64" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D65" s="4">
+      <c r="D65" s="3">
         <v>6</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E65" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="F65" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H65" s="4" t="s">
+      <c r="G65" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H65" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1266,113 +1316,106 @@
       </c>
     </row>
     <row r="71" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D71" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G71" s="3" t="s">
+      <c r="D71" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G71" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H71" s="3" t="s">
+      <c r="H71" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="72" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D72" s="4">
-        <v>1</v>
-      </c>
-      <c r="E72" s="4" t="s">
+      <c r="D72" s="3">
+        <v>1</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F72" s="4" t="s">
+      <c r="F72" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G72" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H72" s="4" t="s">
+      <c r="G72" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H72" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="73" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D73" s="4">
-        <v>2</v>
-      </c>
-      <c r="E73" s="4" t="s">
+      <c r="D73" s="3">
+        <v>2</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F73" s="4" t="s">
+      <c r="F73" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G73" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H73" s="4" t="s">
+      <c r="G73" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H73" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="74" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D74" s="4">
-        <v>3</v>
-      </c>
-      <c r="E74" s="4" t="s">
+      <c r="D74" s="3">
+        <v>3</v>
+      </c>
+      <c r="E74" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F74" s="4" t="s">
+      <c r="F74" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G74" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H74" s="4" t="s">
+      <c r="G74" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H74" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="75" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D75" s="4">
+      <c r="D75" s="3">
         <v>4</v>
       </c>
-      <c r="E75" s="4" t="s">
+      <c r="E75" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F75" s="4" t="s">
+      <c r="F75" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G75" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H75" s="4" t="s">
+      <c r="G75" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H75" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="76" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D76" s="4">
+      <c r="D76" s="3">
         <v>5</v>
       </c>
-      <c r="E76" s="4" t="s">
+      <c r="E76" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F76" s="4" t="s">
+      <c r="F76" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G76" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H76" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
+      <c r="G76" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="79" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C79" s="1" t="s">
@@ -1380,121 +1423,121 @@
       </c>
     </row>
     <row r="82" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D82" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G82" s="3" t="s">
+      <c r="D82" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G82" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H82" s="3" t="s">
+      <c r="H82" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="83" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D83" s="4">
-        <v>1</v>
-      </c>
-      <c r="E83" s="4" t="s">
+      <c r="D83" s="3">
+        <v>1</v>
+      </c>
+      <c r="E83" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F83" s="4" t="s">
+      <c r="F83" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G83" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H83" s="4" t="s">
+      <c r="G83" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H83" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="84" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D84" s="4">
-        <v>2</v>
-      </c>
-      <c r="E84" s="4" t="s">
+      <c r="D84" s="3">
+        <v>2</v>
+      </c>
+      <c r="E84" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F84" s="4" t="s">
+      <c r="F84" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G84" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H84" s="4" t="s">
+      <c r="G84" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H84" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="85" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D85" s="4">
-        <v>3</v>
-      </c>
-      <c r="E85" s="4" t="s">
+      <c r="D85" s="3">
+        <v>3</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F85" s="4" t="s">
+      <c r="F85" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G85" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H85" s="4" t="s">
+      <c r="G85" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H85" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="86" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D86" s="4">
+      <c r="D86" s="3">
         <v>4</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="E86" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F86" s="4" t="s">
+      <c r="F86" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G86" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H86" s="4" t="s">
+      <c r="G86" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H86" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="87" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D87" s="4">
+      <c r="D87" s="3">
         <v>5</v>
       </c>
-      <c r="E87" s="4" t="s">
+      <c r="E87" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F87" s="4" t="s">
+      <c r="F87" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G87" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H87" s="4" t="s">
+      <c r="G87" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H87" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="88" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D88" s="4">
+      <c r="D88" s="3">
         <v>6</v>
       </c>
-      <c r="E88" s="4" t="s">
+      <c r="E88" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F88" s="4" t="s">
+      <c r="F88" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G88" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H88" s="4" t="s">
+      <c r="G88" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H88" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1504,203 +1547,177 @@
       </c>
     </row>
     <row r="95" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D95" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G95" s="3" t="s">
+      <c r="D95" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G95" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H95" s="3" t="s">
+      <c r="H95" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="96" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D96" s="4">
-        <v>1</v>
-      </c>
-      <c r="E96" s="4" t="s">
+      <c r="D96" s="3">
+        <v>1</v>
+      </c>
+      <c r="E96" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F96" s="4" t="s">
+      <c r="F96" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G96" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H96" s="4" t="s">
+      <c r="G96" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H96" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="97" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D97" s="4">
-        <v>2</v>
-      </c>
-      <c r="E97" s="4" t="s">
+      <c r="D97" s="3">
+        <v>2</v>
+      </c>
+      <c r="E97" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F97" s="4" t="s">
+      <c r="F97" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G97" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H97" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="98" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-    </row>
-    <row r="99" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
-      <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
-    </row>
-    <row r="100" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
+      <c r="G97" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="101" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C101" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
     </row>
     <row r="103" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D103" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G103" s="3" t="s">
+      <c r="D103" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G103" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H103" s="3" t="s">
+      <c r="H103" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="104" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D104" s="4">
-        <v>1</v>
-      </c>
-      <c r="E104" s="4" t="s">
+      <c r="D104" s="3">
+        <v>1</v>
+      </c>
+      <c r="E104" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F104" s="4" t="s">
+      <c r="F104" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G104" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H104" s="4" t="s">
+      <c r="G104" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H104" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="105" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D105" s="4">
-        <v>2</v>
-      </c>
-      <c r="E105" s="4" t="s">
+      <c r="D105" s="3">
+        <v>2</v>
+      </c>
+      <c r="E105" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F105" s="4" t="s">
+      <c r="F105" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G105" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H105" s="4" t="s">
+      <c r="G105" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H105" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="106" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D106" s="4">
-        <v>3</v>
-      </c>
-      <c r="E106" s="4" t="s">
+      <c r="D106" s="3">
+        <v>3</v>
+      </c>
+      <c r="E106" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F106" s="4" t="s">
+      <c r="F106" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G106" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H106" s="4" t="s">
+      <c r="G106" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H106" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="107" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D107" s="4">
+      <c r="D107" s="3">
         <v>4</v>
       </c>
-      <c r="E107" s="4" t="s">
+      <c r="E107" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F107" s="4" t="s">
+      <c r="F107" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G107" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H107" s="4" t="s">
+      <c r="G107" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H107" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="108" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D108" s="4">
+      <c r="D108" s="3">
         <v>5</v>
       </c>
-      <c r="E108" s="4" t="s">
+      <c r="E108" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F108" s="4" t="s">
+      <c r="F108" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G108" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H108" s="4" t="s">
+      <c r="G108" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H108" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="109" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D109" s="4">
+      <c r="D109" s="3">
         <v>6</v>
       </c>
-      <c r="E109" s="4" t="s">
+      <c r="E109" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F109" s="4" t="s">
+      <c r="F109" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G109" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H109" s="4" t="s">
+      <c r="G109" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H109" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1710,70 +1727,70 @@
       </c>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D115" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F115" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G115" s="3" t="s">
+      <c r="D115" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G115" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H115" s="3" t="s">
+      <c r="H115" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D116" s="4">
-        <v>1</v>
-      </c>
-      <c r="E116" s="4" t="s">
+      <c r="D116" s="3">
+        <v>1</v>
+      </c>
+      <c r="E116" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F116" s="4" t="s">
+      <c r="F116" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G116" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H116" s="4" t="s">
+      <c r="G116" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H116" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D117" s="4">
-        <v>2</v>
-      </c>
-      <c r="E117" s="4" t="s">
+      <c r="D117" s="3">
+        <v>2</v>
+      </c>
+      <c r="E117" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F117" s="4" t="s">
+      <c r="F117" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G117" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H117" s="4" t="s">
+      <c r="G117" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H117" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D118" s="4">
-        <v>3</v>
-      </c>
-      <c r="E118" s="4" t="s">
+      <c r="D118" s="3">
+        <v>3</v>
+      </c>
+      <c r="E118" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F118" s="4" t="s">
+      <c r="F118" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G118" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H118" s="4" t="s">
+      <c r="G118" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H118" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1783,71 +1800,148 @@
       </c>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D125" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E125" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F125" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G125" s="3" t="s">
+      <c r="D125" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G125" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H125" s="3" t="s">
+      <c r="H125" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="126" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D126" s="4">
-        <v>1</v>
-      </c>
-      <c r="E126" s="4" t="s">
+      <c r="D126" s="3">
+        <v>1</v>
+      </c>
+      <c r="E126" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F126" s="4" t="s">
+      <c r="F126" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G126" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H126" s="4" t="s">
+      <c r="G126" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H126" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="127" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D127" s="4">
-        <v>2</v>
-      </c>
-      <c r="E127" s="4" t="s">
+      <c r="D127" s="3">
+        <v>2</v>
+      </c>
+      <c r="E127" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F127" s="4" t="s">
+      <c r="F127" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G127" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H127" s="4" t="s">
+      <c r="G127" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H127" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="128" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D128" s="4">
-        <v>3</v>
-      </c>
-      <c r="E128" s="4" t="s">
+      <c r="D128" s="3">
+        <v>3</v>
+      </c>
+      <c r="E128" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F128" s="4" t="s">
+      <c r="F128" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G128" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H128" s="4" t="s">
-        <v>9</v>
+      <c r="G128" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D4D2A76-28F4-48B2-8082-1768B10ECBAA}">
+  <dimension ref="F9:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="5">
+        <v>2016</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F11" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="5">
+        <v>2016</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="5">
+        <v>2015</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>